<commit_message>
host docker and edit report
</commit_message>
<xml_diff>
--- a/BAGroup.API/ReportFile/report_speed_violation.xlsx
+++ b/BAGroup.API/ReportFile/report_speed_violation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LAB\BAGroup\WebApi\ReportFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LAB\BAGroup\BAGroup.API\ReportFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -185,6 +185,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -192,15 +201,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -486,79 +486,79 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="1" max="1" width="9.140625" style="10"/>
     <col min="2" max="3" width="15.85546875" style="5" customWidth="1"/>
     <col min="4" max="4" width="27.85546875" style="5" customWidth="1"/>
     <col min="5" max="9" width="9.140625" style="6"/>
     <col min="10" max="10" width="23.5703125" style="4" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="11"/>
-    <col min="13" max="13" width="9.140625" style="12"/>
+    <col min="11" max="12" width="9.140625" style="9"/>
+    <col min="13" max="13" width="9.140625" style="4"/>
     <col min="14" max="14" width="12.140625" style="7" customWidth="1"/>
     <col min="15" max="15" width="13" style="7" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="12"/>
+    <col min="16" max="16" width="9.140625" style="4"/>
     <col min="17" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9" t="s">
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9" t="s">
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
     </row>
     <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
@@ -583,7 +583,7 @@
       <c r="L3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -592,7 +592,7 @@
       <c r="O3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" s="8" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>